<commit_message>
HOMEACC-28: #comment Re-organize data structure #time 3h 0m
</commit_message>
<xml_diff>
--- a/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/DB_Format_Query.xlsx
+++ b/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/DB_Format_Query.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miph272640\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minhphan/PycharmProjects/HomeAccounting/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECF6BEF-4797-4478-9F21-2FAF0AD7BBB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5ECC9BB-CA54-F349-8B26-7B31F282F867}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F55C4BD9-5DD8-4622-A331-6444023C79F7}"/>
+    <workbookView xWindow="11960" yWindow="460" windowWidth="40140" windowHeight="20860" xr2:uid="{F55C4BD9-5DD8-4622-A331-6444023C79F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="117">
   <si>
     <t>Imported</t>
     <phoneticPr fontId="1"/>
@@ -91,10 +91,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>HomeYB_InOut</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>HomeVCB</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -111,10 +107,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>HomeYBVitCard</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Paypay</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -285,24 +277,192 @@
   <si>
     <t>Home Balance (JPY)</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Extendable</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>Vit in Bank (JPY)</t>
+  </si>
+  <si>
+    <t>VitYB</t>
+  </si>
+  <si>
+    <t>Meo in Bank (JPY)</t>
+  </si>
+  <si>
+    <t>MeoYB</t>
+  </si>
+  <si>
+    <t>Yucho Bank Main</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Opt</t>
+  </si>
+  <si>
+    <t>Reminder Only</t>
+  </si>
+  <si>
+    <t>To cross check total balance</t>
+  </si>
+  <si>
+    <t>Yucho Bank Sub</t>
+  </si>
+  <si>
+    <t>Query Expense</t>
+  </si>
+  <si>
+    <t>Query Income</t>
+  </si>
+  <si>
+    <t>Using direction In/Out</t>
+  </si>
+  <si>
+    <t>Q2: reduce "whose"</t>
+  </si>
+  <si>
+    <t>Mom</t>
+  </si>
+  <si>
+    <t>Manual data is designed for Owner -&gt; no need "Whose" field</t>
+  </si>
+  <si>
+    <t>Credit data: still mix there</t>
+  </si>
+  <si>
+    <t>Q22: how to sum and transfer money?</t>
+  </si>
+  <si>
+    <t>Q21: how to cross check with bank deduction?</t>
+  </si>
+  <si>
+    <t>Maybe not necessary, ignore the bank deduction as well</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not base on report file but base on real time data </t>
+  </si>
+  <si>
+    <t>(at anytime check if there is still balance in YB Main then transfer it)</t>
+  </si>
+  <si>
+    <t>Eg: - 300 via bank deduction</t>
+  </si>
+  <si>
+    <t>equal to -100 in YB Main, - 100 in MeoYB, -100 in VitYB then transfer 200 left in YB Main to YB Sub</t>
+  </si>
+  <si>
+    <t>Q23: how about report</t>
+  </si>
+  <si>
+    <t>Not make report file base on input files, but now everything is real time</t>
+  </si>
+  <si>
+    <t>Q24: how aboutitem moved to next month report</t>
+  </si>
+  <si>
+    <t>Real time report do not care this</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q25: how to make sure that no double item </t>
+  </si>
+  <si>
+    <t>(since not fixed report might be imported, and manual input might change)</t>
+  </si>
+  <si>
+    <t>Sol 2-1: Not use database credit anymore but mix credit data to each library</t>
+  </si>
+  <si>
+    <t>Sol 25-1: use middle database to store original record and cross check (time consuming)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sol 25-2: only check for keys: </t>
+  </si>
+  <si>
+    <t>Date, totalPayment to ignore import (show warning and overwrite if needed) (concidence?)</t>
+  </si>
+  <si>
+    <t>Date, totalPayment, Info: still there might be concidence and might double import if Info are wrongly input</t>
+  </si>
+  <si>
+    <t>(so-so)</t>
+  </si>
+  <si>
+    <t>(bad idea)</t>
+  </si>
+  <si>
+    <t>Home Expense</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>Credit DB -&gt; All</t>
+  </si>
+  <si>
+    <t>Home DB -&gt; All</t>
+  </si>
+  <si>
+    <t>1. Filter all item with month and Expense tag</t>
+  </si>
+  <si>
+    <t>2. Then fill to coresponding buffer</t>
+  </si>
+  <si>
+    <t>Home Income</t>
+  </si>
+  <si>
+    <t>1. Filter all item with month and Income tag</t>
+  </si>
+  <si>
+    <t>HomeYB_Main</t>
+  </si>
+  <si>
+    <t>Q2 (cont)</t>
+  </si>
+  <si>
+    <t>How to clean up manual data</t>
+  </si>
+  <si>
+    <t>1. Clear credit payment items</t>
+  </si>
+  <si>
+    <t>2. Sum transfer to/from between 2 YB to 1 transaction</t>
+  </si>
+  <si>
+    <t>3. Copy credit card to DB and check</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -312,13 +472,36 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,6 +562,29 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -389,12 +595,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -434,8 +641,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -748,448 +977,748 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD64953A-B41D-4DCA-BFD7-174DB585D0C9}">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:V49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.25" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="2" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+      <c r="L2" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="L3" t="s">
+        <v>76</v>
+      </c>
+      <c r="N3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4" s="12" t="s">
         <v>6</v>
       </c>
+      <c r="F4" s="12" t="s">
+        <v>5</v>
+      </c>
       <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>104</v>
+      </c>
+      <c r="J4" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C7" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H4" t="s">
+      <c r="G7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I4" t="s">
+      <c r="H7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="K8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="J10" t="s">
-        <v>58</v>
-      </c>
-      <c r="K10" t="s">
-        <v>62</v>
-      </c>
-      <c r="L10" t="s">
-        <v>14</v>
-      </c>
-      <c r="M10" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="N10" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="I7" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="M7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C11" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M11" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+        <v>42</v>
+      </c>
+      <c r="M11" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="M12" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B13" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="J13" t="s">
-        <v>60</v>
-      </c>
-      <c r="K13" t="s">
-        <v>59</v>
-      </c>
-      <c r="L13" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+        <v>44</v>
+      </c>
+      <c r="M13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B14" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" t="s">
+        <v>48</v>
+      </c>
+      <c r="M14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B15" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B16" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" t="s">
-        <v>50</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="B15" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="B16" s="12" t="s">
-        <v>17</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+        <v>46</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B17" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>98</v>
+      </c>
+      <c r="R17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B18" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>99</v>
+      </c>
+      <c r="R18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B19" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="L19" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="M20" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B21" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
       </c>
-      <c r="D21" t="s">
-        <v>22</v>
+      <c r="D21" s="10" t="s">
+        <v>68</v>
       </c>
       <c r="E21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+        <v>46</v>
+      </c>
+      <c r="K21" t="s">
+        <v>56</v>
+      </c>
+      <c r="L21" t="s">
+        <v>60</v>
+      </c>
+      <c r="M21" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="N21" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O21" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>58</v>
+      </c>
+      <c r="R21" t="s">
+        <v>57</v>
+      </c>
+      <c r="S21" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="U21" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>13</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="N22" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="O22" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="S22" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B23" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="E23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="L23">
+        <v>9999</v>
+      </c>
+      <c r="M23">
+        <v>888</v>
+      </c>
+      <c r="N23">
+        <v>777</v>
+      </c>
+      <c r="O23">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>53</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" t="s">
+        <v>26</v>
+      </c>
+      <c r="K25" t="s">
+        <v>56</v>
+      </c>
+      <c r="L25" t="s">
+        <v>63</v>
+      </c>
+      <c r="M25" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>69</v>
+      </c>
+      <c r="R25" t="s">
+        <v>67</v>
+      </c>
+      <c r="S25" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="T25" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="U25" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>54</v>
       </c>
-      <c r="E24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B26" t="s">
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" t="s">
+        <v>26</v>
+      </c>
+      <c r="L26">
+        <v>8888</v>
+      </c>
+      <c r="M26" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="S26" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="T26" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="R27">
+        <v>9999</v>
+      </c>
+      <c r="S27">
+        <v>888</v>
+      </c>
+      <c r="T27">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="C28" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K28" t="s">
         <v>56</v>
       </c>
-      <c r="C26" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="C28" s="3" t="s">
+      <c r="L28" t="s">
+        <v>65</v>
+      </c>
+      <c r="M28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="C29" t="s">
+      <c r="L29">
+        <v>7777</v>
+      </c>
+      <c r="M29" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>69</v>
+      </c>
+      <c r="R29" t="s">
+        <v>72</v>
+      </c>
+      <c r="S29" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="T29" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="U29" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="V29" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>34</v>
+      </c>
+      <c r="S30" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="T30" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="U30" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
         <v>27</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D31" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="C30" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="R31">
+        <v>9999</v>
+      </c>
+      <c r="S31">
+        <v>888</v>
+      </c>
+      <c r="T31">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="C31" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" t="s">
+    <row r="33" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="C32" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" t="s">
+    <row r="34" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.4">
-      <c r="C33" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="L34" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.4">
-      <c r="C34" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.4">
-      <c r="C35" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35" t="s">
-        <v>41</v>
+      <c r="J35" t="s">
+        <v>101</v>
+      </c>
+      <c r="K35" t="s">
+        <v>100</v>
+      </c>
+      <c r="L35" t="s">
+        <v>105</v>
+      </c>
+      <c r="N35" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="L36" t="s">
+        <v>106</v>
+      </c>
+      <c r="N36" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="L39" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="J40" t="s">
+        <v>101</v>
+      </c>
+      <c r="K40" t="s">
+        <v>109</v>
+      </c>
+      <c r="L40" t="s">
+        <v>106</v>
+      </c>
+      <c r="N40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="N41" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="L46" t="s">
+        <v>112</v>
+      </c>
+      <c r="M46" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="M47" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="M48" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M49" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HOMEACC-28: #comment Re-organize clean up #time 0h 10m
</commit_message>
<xml_diff>
--- a/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/DB_Format_Query.xlsx
+++ b/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/DB_Format_Query.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minhphan/PycharmProjects/HomeAccounting/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5ECC9BB-CA54-F349-8B26-7B31F282F867}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F718367-0443-934E-ADB1-FBC1FBB627C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11960" yWindow="460" windowWidth="40140" windowHeight="20860" xr2:uid="{F55C4BD9-5DD8-4622-A331-6444023C79F7}"/>
+    <workbookView xWindow="7300" yWindow="2160" windowWidth="40140" windowHeight="20860" xr2:uid="{F55C4BD9-5DD8-4622-A331-6444023C79F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -980,7 +980,7 @@
   <dimension ref="A1:V49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
HOMEACC-28: #comment Format and Query #time 0h 10m #description Design Database
</commit_message>
<xml_diff>
--- a/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/DB_Format_Query.xlsx
+++ b/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/DB_Format_Query.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minhphan/PycharmProjects/HomeAccounting/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miph272640\PycharmProjects\HomeAccounting\trial\MeoDemo_Final\Prepare_Manual\SpreadSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F718367-0443-934E-ADB1-FBC1FBB627C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CDBCD1-AD04-4D52-B049-BF26EAD27261}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7300" yWindow="2160" windowWidth="40140" windowHeight="20860" xr2:uid="{F55C4BD9-5DD8-4622-A331-6444023C79F7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{F55C4BD9-5DD8-4622-A331-6444023C79F7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Master" sheetId="1" r:id="rId1"/>
+    <sheet name="AccountSummary" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="125">
   <si>
     <t>Imported</t>
     <phoneticPr fontId="1"/>
@@ -445,6 +446,38 @@
   </si>
   <si>
     <t>3. Copy credit card to DB and check</t>
+  </si>
+  <si>
+    <t>cycle</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DBName</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Home Balance</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Vit In Bank</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Meo In Bank</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Yucho 1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Yucho 2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HomeYB_Main</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -455,14 +488,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -472,7 +505,7 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -480,14 +513,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -496,12 +529,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -585,6 +618,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -601,7 +640,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -660,6 +699,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -979,38 +1021,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD64953A-B41D-4DCA-BFD7-174DB585D0C9}">
   <dimension ref="A1:V49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView topLeftCell="G10" zoomScale="119" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19:U31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" customWidth="1"/>
+    <col min="8" max="8" width="10.125" customWidth="1"/>
+    <col min="10" max="10" width="13.125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
@@ -1021,7 +1063,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
@@ -1035,7 +1077,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -1063,16 +1105,19 @@
       <c r="J4" t="s">
         <v>49</v>
       </c>
+      <c r="K4" s="20" t="s">
+        <v>117</v>
+      </c>
       <c r="N4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
       <c r="M5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -1083,7 +1128,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
       <c r="C7" s="17" t="s">
         <v>102</v>
       </c>
@@ -1112,22 +1157,25 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
       <c r="P9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
       <c r="P10" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="B11" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="C11" s="2" t="s">
         <v>23</v>
       </c>
@@ -1147,7 +1195,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1173,7 +1221,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B13" s="12" t="s">
         <v>14</v>
       </c>
@@ -1193,7 +1241,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B14" s="12" t="s">
         <v>15</v>
       </c>
@@ -1216,7 +1264,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B15" s="12" t="s">
         <v>32</v>
       </c>
@@ -1239,7 +1287,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B16" s="12" t="s">
         <v>16</v>
       </c>
@@ -1259,7 +1307,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.4">
       <c r="B17" s="12" t="s">
         <v>17</v>
       </c>
@@ -1282,7 +1330,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.4">
       <c r="B18" s="12" t="s">
         <v>41</v>
       </c>
@@ -1305,7 +1353,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.4">
       <c r="B19" s="12" t="s">
         <v>18</v>
       </c>
@@ -1325,7 +1373,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1351,7 +1399,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.4">
       <c r="B21" s="12" t="s">
         <v>20</v>
       </c>
@@ -1395,7 +1443,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1427,7 +1475,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.4">
       <c r="B23" s="12" t="s">
         <v>22</v>
       </c>
@@ -1456,24 +1504,30 @@
         <v>666</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
         <v>51</v>
       </c>
       <c r="C24" t="s">
         <v>52</v>
       </c>
+      <c r="D24" t="s">
+        <v>51</v>
+      </c>
       <c r="E24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
         <v>53</v>
       </c>
       <c r="C25" t="s">
         <v>52</v>
       </c>
+      <c r="D25" t="s">
+        <v>53</v>
+      </c>
       <c r="E25" t="s">
         <v>26</v>
       </c>
@@ -1502,13 +1556,16 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
         <v>54</v>
       </c>
       <c r="C26" t="s">
         <v>52</v>
       </c>
+      <c r="D26" t="s">
+        <v>54</v>
+      </c>
       <c r="E26" t="s">
         <v>26</v>
       </c>
@@ -1525,7 +1582,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.4">
       <c r="R27">
         <v>9999</v>
       </c>
@@ -1536,7 +1593,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.4">
       <c r="C28" s="3" t="s">
         <v>31</v>
       </c>
@@ -1553,7 +1610,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.4">
       <c r="C29" t="s">
         <v>25</v>
       </c>
@@ -1585,7 +1642,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.4">
       <c r="C30" t="s">
         <v>30</v>
       </c>
@@ -1602,7 +1659,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.4">
       <c r="C31" t="s">
         <v>27</v>
       </c>
@@ -1619,7 +1676,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.4">
       <c r="C32" t="s">
         <v>29</v>
       </c>
@@ -1627,7 +1684,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C33" t="s">
         <v>17</v>
       </c>
@@ -1635,7 +1692,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C34" t="s">
         <v>20</v>
       </c>
@@ -1646,7 +1703,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C35" t="s">
         <v>22</v>
       </c>
@@ -1666,7 +1723,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:14" x14ac:dyDescent="0.4">
       <c r="L36" t="s">
         <v>106</v>
       </c>
@@ -1674,12 +1731,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:14" x14ac:dyDescent="0.4">
       <c r="L39" s="15" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:14" x14ac:dyDescent="0.4">
       <c r="J40" t="s">
         <v>101</v>
       </c>
@@ -1693,12 +1750,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:14" x14ac:dyDescent="0.4">
       <c r="N41" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:14" x14ac:dyDescent="0.4">
       <c r="L46" t="s">
         <v>112</v>
       </c>
@@ -1706,17 +1763,17 @@
         <v>113</v>
       </c>
     </row>
-    <row r="47" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:14" x14ac:dyDescent="0.4">
       <c r="M47" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:14" x14ac:dyDescent="0.4">
       <c r="M48" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="13:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M49" t="s">
         <v>116</v>
       </c>
@@ -1724,5 +1781,272 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{669DE897-8056-44FC-B1CD-428F3D45220D}">
+  <dimension ref="B2:L27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="3" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:11" x14ac:dyDescent="0.4">
+      <c r="C2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2">
+        <v>9999</v>
+      </c>
+      <c r="G2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H2">
+        <v>9999</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="3" spans="3:11" x14ac:dyDescent="0.4">
+      <c r="C3" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3">
+        <v>6666</v>
+      </c>
+      <c r="G3" t="s">
+        <v>121</v>
+      </c>
+      <c r="H3">
+        <v>6666</v>
+      </c>
+      <c r="J3" t="s">
+        <v>122</v>
+      </c>
+      <c r="K3">
+        <v>8888</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.4">
+      <c r="C4" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4">
+        <v>2222</v>
+      </c>
+      <c r="J4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K4">
+        <v>7777</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.4">
+      <c r="C5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>1111</v>
+      </c>
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5">
+        <v>6666</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.4">
+      <c r="C15" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.4">
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" t="s">
+        <v>57</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="D18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C19">
+        <v>9999</v>
+      </c>
+      <c r="D19">
+        <v>888</v>
+      </c>
+      <c r="E19">
+        <v>777</v>
+      </c>
+      <c r="F19">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" t="s">
+        <v>64</v>
+      </c>
+      <c r="H21" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21" t="s">
+        <v>67</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L21" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C22">
+        <v>8888</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="I23">
+        <v>9999</v>
+      </c>
+      <c r="J23">
+        <v>888</v>
+      </c>
+      <c r="K23">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C25">
+        <v>7777</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" t="s">
+        <v>69</v>
+      </c>
+      <c r="I25" t="s">
+        <v>72</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="K25" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="L25" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="J26" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K26" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L26" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="I27">
+        <v>9999</v>
+      </c>
+      <c r="J27">
+        <v>888</v>
+      </c>
+      <c r="K27">
+        <v>777</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>